<commit_message>
Site updated: 2019-06-05 18:16:48
</commit_message>
<xml_diff>
--- a/2019/06/03/数据库20190603/example_prime_attr.xlsx
+++ b/2019/06/03/数据库20190603/example_prime_attr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACM\Blog\medioqrity.github.io\blog\source\_posts\数据库20190603\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBEED52-C59F-4C69-A75C-4C6480B43D9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77608B74-A050-4723-A7C2-AE2E309186E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{5BEF7453-338B-4621-BAAD-90377BEE951A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>房间号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,6 +61,34 @@
   </si>
   <si>
     <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dcount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -148,8 +176,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -481,85 +512,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E12942-EF9A-4CC0-B351-BDF27A0EBD76}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I12" sqref="I12:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.899999999999999" x14ac:dyDescent="0.8"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.8">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.8">
-      <c r="A3" s="4" t="s">
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>316</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.8">
-      <c r="A4" s="4" t="s">
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>101</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>150</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.8">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>400</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.8">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>207</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.8">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>810</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>1919</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>140</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1">
+        <v>140</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>140</v>
+      </c>
+      <c r="I13" s="1">
+        <v>140</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1">
+        <v>140</v>
+      </c>
+      <c r="I14" s="1">
+        <v>140</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>